<commit_message>
Data Input Menu and Help Pages added
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R9495445b46084bd2"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R4f16c34d8acd4756"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R2b6d8ed3421d4661"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R26ca35d17da0414c"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{775801b2-0cd3-40d2-8184-f18d8c837ae8}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{af5830dd-a268-4700-9d20-08a0084c0b06}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Broke it so I fixed it
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R9c669d81a4404b9f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R9bbe6a6ffb6e4264"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R664f04c5be7941e3"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re34fd6bb0de8442e"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{98600f37-fc01-4e11-92ff-bdbaeac9a5f5}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{8d30e22f-204d-4f5e-bab5-1b200c9e11b4}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
letters to numbers function
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R139b725c677a4af6"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rde19206f69a34e23"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R4407484a2ff143cb"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R77727ff7b1124ba4"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{700e1abe-c771-4e90-8528-521707e1ba72}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{39dcfb9c-717c-4bee-86ca-852fa39f57fd}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Nigel you were right my bad. Left one last comment on it though
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R2f735a66545b4cba"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Ref69db3d393f43e8"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R23e701dc789c4537"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rd8e7268020ac4f63"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{0fc78f48-08dc-4fb0-9ae8-bcf10a22ec94}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{a94c1b05-fa5e-48d5-aee2-7b5a57e9a392}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Started saved search UI
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Ref69db3d393f43e8"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R7dddb6d616a4420b"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rd8e7268020ac4f63"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rb27c68154667434d"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{a94c1b05-fa5e-48d5-aee2-7b5a57e9a392}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{9400b201-5e1c-465b-9b22-b414bfa18487}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Added new functions, noting is linked in yet and so not tested (wont break anything though app still opens). Also realised we will need to do seperate js pages for each of the U.I. pages and this means we need a way to pass data between the pages. Will work on this later and re-organise js file (i.e. add more)
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Ref69db3d393f43e8"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R643a19e3a46b4878"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rd8e7268020ac4f63"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R9ae1d63a298a4a48"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{a94c1b05-fa5e-48d5-aee2-7b5a57e9a392}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{5dfba861-649f-49e0-a9c3-8bf5502b4b6e}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Working on changing search type page
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R7dddb6d616a4420b"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rf69aa1a0cfa340d6"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rb27c68154667434d"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R41bc453780eb495d"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{9400b201-5e1c-465b-9b22-b414bfa18487}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{cfe6f697-b0c0-4cd0-b300-d6c70b725a18}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
ok, so this is a pretty big change... I've got all mark's changes in here plus I made some pretty big ones myself... need to talk to everyone working with the html at the next meeting since some of the things that are being copied and pasted are breaking the js. Also appologies for any bugs or stuff in this I know it is rough but at least it returns something on searches so we can show it working on tuesday. Also have to change the search so it will ignore white space.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R7dddb6d616a4420b"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R88a59201e2384417"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rb27c68154667434d"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R40f7e3cdd032426b"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{9400b201-5e1c-465b-9b22-b414bfa18487}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{44998f1c-18ae-45e9-b502-69eff566cef9}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Hey guys. Just got back from my trip and have only been able to work on this tonight. I did a couple things here. First I separated the range selection and data input. Second I added a canvas that tells the user what column they entered (will look better later). Third I added some dynamic buttons so that the user can add information one piece at a time not needing to use commas.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rd447b62cef2049f2"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R59e9284a9c544ca0"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R0bfa54b822734694"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R879c590bb9734021"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{874c7bfc-83fa-4679-bebc-55e24af13289}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{224d5895-7945-4e4c-8fe4-c5f5c75254a0}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
trying to add things to exclude
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rd447b62cef2049f2"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rae8da79043c24f36"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R0bfa54b822734694"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Radb30220f29d44eb"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{874c7bfc-83fa-4679-bebc-55e24af13289}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{b65dc72b-5c54-45bd-bb94-9ed4780adb8a}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
buttons added, compatible with backend
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rd447b62cef2049f2"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R96898b5076ec4d61"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R0bfa54b822734694"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R7d618e623a5b40c8"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{874c7bfc-83fa-4679-bebc-55e24af13289}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{71e61a68-663a-4cd8-a270-e9ef6625b218}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Made a function searchToString() which should create a string which contains the formatted search details. I'm not sure how to actually print it as text though
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R6396203441134469"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R445830df252c418d"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R9f70d8cd3d394c81"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R295553669f3846da"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{bc333373-1f4e-4008-8070-39f04c1dd4e7}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{d8aec38b-dcf9-4d0a-b4f1-c4d21084b2b4}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
fixed for one variable search
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R445830df252c418d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rffe868a76d544ac4"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R295553669f3846da"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R62c0d9cf2ddb4ea3"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{d8aec38b-dcf9-4d0a-b4f1-c4d21084b2b4}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{97d55f29-a9cc-47c8-a522-8c47ec8653d8}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Thea great job with the errors and it seems that the popup return type idea has legs. Just added a quick additional check to make sure that the column input is of valid characters. I'm at a tournament in Galway till Thursday but should get to implement the input menu by the end of the week.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rffe868a76d544ac4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rcc3cce32ae794274"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R62c0d9cf2ddb4ea3"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Ra545fc1dbf0e4123"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{97d55f29-a9cc-47c8-a522-8c47ec8653d8}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{fcdc61ac-eb8d-4a7c-b639-2a35b41878ae}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
silly git... i haven't done anything
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rffe868a76d544ac4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R41f62b3e51834653"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R62c0d9cf2ddb4ea3"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R696989db2b3b4742"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{97d55f29-a9cc-47c8-a522-8c47ec8653d8}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{53e0d5c9-192f-42c3-b19c-0c567d7a16a9}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Fixed it so it reads in dates right :)
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R41f62b3e51834653"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R82d238dee50d4de8"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R696989db2b3b4742"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R8904ca84bde04e5c"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{53e0d5c9-192f-42c3-b19c-0c567d7a16a9}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{7b29491d-8aa2-4630-9c57-e26c37727d30}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
searches save mostly, don't load yet though
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R82d238dee50d4de8"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re23fe770ff6f4ef8"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R8904ca84bde04e5c"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R48decee9452d4551"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{7b29491d-8aa2-4630-9c57-e26c37727d30}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{dcdfcdad-c948-4c7a-9957-4ec7dddcbb2d}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
searches load but only seem to save per session (i.e. close the app and they are gone) but i dont know if this is just because we are running in debug mode or not. Going to test this now.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re23fe770ff6f4ef8"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R6cc7c1a9b12049b7"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R48decee9452d4551"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R753a84afede4475e"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{dcdfcdad-c948-4c7a-9957-4ec7dddcbb2d}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{43c559bb-2121-4096-ad3d-0fd90db223b6}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Dan, just moved your new check, it wasn't getting called where it was :P
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R6cc7c1a9b12049b7"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rbaaf57934535497f"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R753a84afede4475e"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R32602979ab6447ef"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{43c559bb-2121-4096-ad3d-0fd90db223b6}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4119bbdc-1088-4cb2-aea1-33e6fc1a2d07}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
changing the input menu
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rbaaf57934535497f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R2c260b076e8f44aa"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R32602979ab6447ef"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rf4714fda97a3431b"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4119bbdc-1088-4cb2-aea1-33e6fc1a2d07}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{b4cc3226-725b-4233-8bb8-d0f25614f671}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
working on range. don't use for now -- to be completed when I am less tired
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R2c260b076e8f44aa"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rc8556d8ab803485f"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rf4714fda97a3431b"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R819136dec0324f11"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{b4cc3226-725b-4233-8bb8-d0f25614f671}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{7dfa6d65-38ef-4094-a715-824cd33f50f9}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Trying to make UI as simple as possible for the non-technical user. This does not work fully but it is going toward a simpler UI.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rc8556d8ab803485f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R921b4bf7f85b44f9"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R819136dec0324f11"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5445d75089024ea7"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{7dfa6d65-38ef-4094-a715-824cd33f50f9}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{7e044236-d5dc-4940-8607-73cd6ea4b1f5}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
simpler ui-will demo at mtg
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R921b4bf7f85b44f9"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Ra0e1f37c886e4a7a"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5445d75089024ea7"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R3314753e540c4382"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{7e044236-d5dc-4940-8607-73cd6ea4b1f5}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{889a6c40-8c36-4d60-91c4-9795aa36ff2f}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
still working on simpler ui
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R114b3a5f102b43c4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R5346b486d46c4e1a"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R02cf5fc340494f6c"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R67b28ccf061549b8"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{2432e1ca-5485-46bf-98b9-d2055d1638f5}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{e56bf192-fe8c-49bf-b655-9954012edd78}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
more work on UI, merged mark's gif, took out useless menu at end. Small problem with removing dynamic buttons if they just contain integer value but easily fixable. Merging is done people can now add to this master branch no problem.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Reb9f3aa1e6f346dc"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R661d21b35a60481b"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R58734557c5144e93"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rc13d38fdbffb48ea"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{bff3d839-15cc-4c2c-9b67-e435f98852cf}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{a654d7f7-39a9-4c60-97c9-faa97e11af2f}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
ui stuff, marks gif added, took out useless menu
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R661d21b35a60481b"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R7733e0c322694c7d"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rc13d38fdbffb48ea"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rb0980cb7197a4181"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{a654d7f7-39a9-4c60-97c9-faa97e11af2f}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{bd5db51a-e30f-4b23-8036-fe91a390b018}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Changed a lot of the wording, and added a bindings page.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R7733e0c322694c7d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rc66b16ece77d4d73"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rb0980cb7197a4181"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rfb425553d24a457c"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{bd5db51a-e30f-4b23-8036-fe91a390b018}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{34329fa5-b829-406f-a3bd-a2671775b6b8}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
mouse automatically activates in next text box to minimize clicking. next step -- hook up search summary deletion to backend and display red x/brief text when hovering over buttons
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R9153252556fa4ce7"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rf007c12ee3464281"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rf55a0cc378e34441"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R37631732f75e4c5d"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{d07888bf-6f1b-4966-a5f8-3c19e6eaa903}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{7fd85190-af93-479d-bd9a-8c831af174c5}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Messing with css on headings
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rc66b16ece77d4d73"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R9153252556fa4ce7"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rfb425553d24a457c"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rf55a0cc378e34441"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{34329fa5-b829-406f-a3bd-a2671775b6b8}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{d07888bf-6f1b-4966-a5f8-3c19e6eaa903}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Changed the bindings page. Added a tutorial page which runs through everything. It has pictures but I change them and add more once we are settled on the design. Fixed some navigation buttons throughout the app.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rf007c12ee3464281"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R95ff085b735541b9"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R37631732f75e4c5d"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5cb4a420464148e1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{7fd85190-af93-479d-bd9a-8c831af174c5}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1ad61dc4-45db-4197-b9fd-f71ec5ffe11f}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
removed pop up for column search value entry
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R95ff085b735541b9"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R96b1af04a553409a"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5cb4a420464148e1"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rd482534708554f23"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1ad61dc4-45db-4197-b9fd-f71ec5ffe11f}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{ab904afb-a54d-4e65-9c2e-76aec37a9404}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
stopped pop up cause it is slow
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R96b1af04a553409a"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R2fc3466c987049d9"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rd482534708554f23"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R64fb402b6ec84f44"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{ab904afb-a54d-4e65-9c2e-76aec37a9404}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{0a667c94-e0eb-4d24-bec7-34c6d11891fc}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
search is now saved after being run
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R2fc3466c987049d9"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R28931151c7e7475f"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R64fb402b6ec84f44"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R7f34a598a2b64b0d"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{0a667c94-e0eb-4d24-bec7-34c6d11891fc}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{c8ab9b97-261e-4ca6-8c38-7db8de0de1d0}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
quick fix to button that was bugging me
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re0c79aaddc4644a1"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rc40bf584e3e14f56"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R111ee02ec1084a43"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R4a930cb876cd4996"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{bd016427-830b-40cf-867f-2b4cfee0cbef}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{16e2ab2d-fe7e-4c5e-87d3-4fba4273fc34}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
messing around with css. Let me know what you think. really easy to change back and wont be offended at all if you all hate it :P
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R28931151c7e7475f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re0c79aaddc4644a1"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R7f34a598a2b64b0d"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R111ee02ec1084a43"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{c8ab9b97-261e-4ca6-8c38-7db8de0de1d0}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{bd016427-830b-40cf-867f-2b4cfee0cbef}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
error messages align left
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R1869de0178db4407"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R1e69a7bded614791"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R9fd6cdb689b94f95"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R72b37e2d4a164f6a"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{8a67fe00-616f-4070-aae6-011205df3c87}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1381032f-ebf8-4612-9a02-219f93fb647c}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
changed col entry button size to avoid confusion
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Ra7198b8a8c054a3b"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rdd60033ddf9f4b55"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R662eea9844e54e23"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Ra04c811bb72f4403"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{458afc53-70b6-4b54-94a1-43a59fdd43d8}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{48dd5799-35ec-435c-9b15-7a24c9852238}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
added cookies to track user's first time on the app and open tutorial automatically on the first time. Not sure if it works with the published version but I will check.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rdd60033ddf9f4b55"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R27c4d498b8644d1e"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Ra04c811bb72f4403"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R8adba0c4925042c0"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{48dd5799-35ec-435c-9b15-7a24c9852238}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{52047c0e-dcc2-4391-9dfb-8c7554b27cc5}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Added some error messages. Will have to do some work on the case when the search does not return any data. I'm envisioning that the user would be able to go back and change the search parameters. Great work on the return type nigel -- we have a little time to work out the bugs.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R27c4d498b8644d1e"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R6ae69b0ad7be4123"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R8adba0c4925042c0"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rde16d69c4e6144ab"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{52047c0e-dcc2-4391-9dfb-8c7554b27cc5}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{9e34e415-bcf4-416b-a8c5-3dbab648763b}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Displaying in rows, but not fully working still.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rf169797c8246427d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rc393bcf37b064b85"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R4584082b8d554563"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R995f5eafcc724c05"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4cb5caf6-f0a0-4006-9030-c302b12c707e}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{d58ea47d-8a90-46fd-b3d6-f106417d8a25}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
making some fairly big changes. can people hold off on commits for the next 30 mins or so.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rc393bcf37b064b85"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R1ee731978d1945b2"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R995f5eafcc724c05"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re3ac11a6b31c4a13"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{d58ea47d-8a90-46fd-b3d6-f106417d8a25}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4a95b9d5-2062-42b3-aab4-c40b61ef0871}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
OK a fairly big change to UI in terms of error catching here. If the user runs a search that doesn't return anything, they are directed to Oops.html, where they can either modify the search they just ran (ideally) or start over. The big change comes in the backend where I actually run the search in NewSearch.js to see if there are any results and if there are I store them in localsto
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R1ee731978d1945b2"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R1c4c6a28d1944aae"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re3ac11a6b31c4a13"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R7ef0334ea13d4aff"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4a95b9d5-2062-42b3-aab4-c40b61ef0871}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{eebe115d-a781-4345-b99c-2f57533ad4cf}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
save button hidden when no searches saved
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R530d6bca194a4695"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Ra6a3747b132e46f8"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rd0c907595b2b4441"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rad17c8b91e2f405a"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{d89bf0cb-3842-4df4-a378-34cbce25f226}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{8cd9f935-22d8-4b10-89e8-a398916a6126}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Hooked up the sheet entry to the backend. We are on the home stretch here team.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rb12ba5b3a6bb4ebc"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re5c9ae0541a74b92"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R58e21a7b2c284cc1"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R95110f7dfb634305"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{b7abe915-e947-4fba-957e-c94e3457b5af}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{dcfeef7b-c40c-41ba-b5cd-4c2fb312d45d}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Got Nigel's output to display in the right way. I think we can submit this thing unless there are any objections.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re5c9ae0541a74b92"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R2d4d248c7a574f5d"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R95110f7dfb634305"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rbb43955f245b470b"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{dcfeef7b-c40c-41ba-b5cd-4c2fb312d45d}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{a1035496-aa7e-4e6f-a2d7-4ab9be3158a7}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
fix to allow data to be shown in more than 26 cols if need be.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R2d4d248c7a574f5d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rc395061d1e7641a1"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rbb43955f245b470b"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R4ce220ad201d4949"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{a1035496-aa7e-4e6f-a2d7-4ab9be3158a7}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{509c94b6-6459-4a40-886c-018fbabefcac}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Slight wording change. Sample toggle button for range
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R6d91b26649384345"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R721bae370978431d"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rcbaaf7205d1c42a0"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rdd8d7e3797d44579"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{f793bddf-b79a-4c14-9762-39e7b725d619}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1086f244-e357-40b8-bd52-e67892fcd3e5}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Tidied up error messages and removed toggle button
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R721bae370978431d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rc027420ed3f84557"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rdd8d7e3797d44579"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R97f19fd898e74a29"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1086f244-e357-40b8-bd52-e67892fcd3e5}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{c47ead94-70b9-46ce-801b-b449afd39960}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
took bad loop out of output, should run faster now. Deleted a bunch of code that we don't use. Got it to remove a search term by clicking on it.
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rcf43def740ad43ce"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rbccfb77c9291408f"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R50f9d2d5b84b4383"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R84d1a2bc8cff4370"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{43a81f95-5c2e-45f3-84ca-b09de6cdf5e1}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{c6dcf9e7-f348-4dca-8280-6e87f8773316}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
images over search elements
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R1fe0c336cb7a4782"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rcf43def740ad43ce"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rc473da2b17794c2e"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R50f9d2d5b84b4383"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{3c86aab4-9393-40f6-91be-ed47d428ef3c}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{43a81f95-5c2e-45f3-84ca-b09de6cdf5e1}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Fixed internet stuff and double return values stuff
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R48331e8bd5244f55"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R2ed15ad25f5c43ae"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R6b668b1e777b4d2d"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rde452bbd7d894f59"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{901f31da-1f22-49b1-863f-0cc7981960b8}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{513ffdc0-cc81-4b96-8e6b-739a5a4b73f3}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
changed home to cancel
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rd6b270f7564d4d79"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rdf81e7b09f904561"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R4b36bffcf7c24292"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rfcc3514b57104a60"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{82f3ea27-c582-4d0e-bc13-582d348f59c7}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{27d0119f-28d3-474c-a8f9-34a997c5257e}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Save search details working... but currently being displayed as an error message. Still working at printing them in a div
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rbc7010e17e09472a"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R9bbae722833e48c9"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rffc195fc19b24c7e"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Raf28200f42c04db2"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{e8a3d38a-0c0d-4f97-9897-95cb34917a34}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{c634f983-d17e-4bc3-8013-3d9c54c0135e}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
still tring to fix serch details display
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R9bbae722833e48c9"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R5899db91765a447d"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Raf28200f42c04db2"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R881a281f76b14858"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{c634f983-d17e-4bc3-8013-3d9c54c0135e}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{61c32b76-c833-44da-a835-d3f58bc7437c}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Caught a standard error message in bindings, made it more understandable for users
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R5899db91765a447d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Ra76a4b1960434293"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R881a281f76b14858"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rfe25c38bbd1f4ab0"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{61c32b76-c833-44da-a835-d3f58bc7437c}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{cbb7c844-323b-49b0-a29c-bbe481cf34df}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
i ran it or something
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R7838063aed464363"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rda96bb35f12a4e65"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R4a493d0ee293418f"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R96a3c7479f8c412c"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{7907d8e0-c886-4c6f-94dc-9207edf1cb06}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{bd0e77c0-e80d-409d-b04a-f50abb10edf5}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Fixed spaces issue (by putting in an error message)
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Ra76a4b1960434293"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R3bea88effc07431f"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rfe25c38bbd1f4ab0"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R8e24fa12a1914279"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{cbb7c844-323b-49b0-a29c-bbe481cf34df}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{e2878bde-22a6-4a2c-bd3c-b0f264dd4b14}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Think i fixed the ie9 problem...
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R3bea88effc07431f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rf89e749a4d4342ec"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R8e24fa12a1914279"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R39c553d2e12943b3"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{e2878bde-22a6-4a2c-bd3c-b0f264dd4b14}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{ac9e6e6c-b5dc-4b6a-8ae1-053f8baa0759}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
View save search details now working
</commit_message>
<xml_diff>
--- a/monstrApp/monstrApp/bin/Debug/Book1.xlsx
+++ b/monstrApp/monstrApp/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rdf81e7b09f904561"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R22f1451365364e25"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rfcc3514b57104a60"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R3ff88ae2e5204371"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{27d0119f-28d3-474c-a8f9-34a997c5257e}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{a682bd93-dab1-457d-b43c-62de865f2bd9}">
   <we:reference id="76ced0e3-ef80-4b7e-af22-0934be9fe3f1" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>